<commit_message>
aggiunto uml model mvc
</commit_message>
<xml_diff>
--- a/uml/ObserverMessage.xlsx
+++ b/uml/ObserverMessage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\IdeaProjects\ing-sw-2020-romeo-pozzan-prada\uml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D23E803-6EC1-41D2-946E-6E4B7706A207}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458AF523-6FF0-4A66-9BCE-2CE2960AECAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CDE221DC-C4BE-42D4-8A58-4F7DBA3DE5B2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>PLAYER_ACTION</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>NotifyNotYourTurn</t>
+  </si>
+  <si>
+    <t>called by function</t>
   </si>
 </sst>
 </file>
@@ -159,7 +162,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,8 +181,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -187,15 +196,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -510,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4168E1C6-7DF1-4307-8722-73093556EEE6}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,22 +551,40 @@
     <col min="3" max="4" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="38.140625" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" customWidth="1"/>
+    <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="36.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="J1" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -560,23 +606,29 @@
       <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="J3" t="s">
+      <c r="I3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" t="s">
         <v>18</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>19</v>
-      </c>
-      <c r="L3" t="s">
-        <v>20</v>
       </c>
       <c r="M3" t="s">
         <v>20</v>
       </c>
       <c r="N3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -598,140 +650,145 @@
       <c r="G5" t="s">
         <v>7</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>1</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>11</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>12</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>13</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="2"/>
-      <c r="J6" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="3"/>
+      <c r="K6" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="1"/>
-      <c r="P6" t="s">
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="4"/>
+      <c r="Q6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="J7" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="K7" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="1"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="1"/>
-      <c r="P7" t="s">
+      <c r="L7" s="4"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="4"/>
+      <c r="Q7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="J8" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="K8" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="P8" t="s">
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="Q8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="J9" t="s">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="K9" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="1"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="2"/>
-      <c r="P9" t="s">
+      <c r="L9" s="4"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="3"/>
+      <c r="Q9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="J10" t="s">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
         <v>26</v>
       </c>
-      <c r="K10" s="1"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="1"/>
-      <c r="P10" t="s">
+      <c r="L10" s="4"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="4"/>
+      <c r="Q10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="J11" t="s">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="1"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="P11" t="s">
+      <c r="L11" s="4"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="Q11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="J12" t="s">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
         <v>28</v>
       </c>
-      <c r="K12" s="1"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="1"/>
-      <c r="P12" t="s">
+      <c r="L12" s="4"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="4"/>
+      <c r="Q12" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="K1:Q1"/>
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>